<commit_message>
Added .gitignore to root, started UI-testing and added Testrapport.docx
</commit_message>
<xml_diff>
--- a/Documentation/Testplanering_Testfall.xlsx
+++ b/Documentation/Testplanering_Testfall.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Local\Peter\Testning\SecuremeTesting@fendraq\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3983C48D-E867-467C-BA7A-0882645972B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BFCE26F-7AED-4C6E-BB58-741890DF2A95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" firstSheet="2" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="187">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="213">
   <si>
     <t>Test-ID</t>
   </si>
@@ -467,9 +467,6 @@
     <t>Fälten validerar korrekt input och visar felmeddelanden</t>
   </si>
   <si>
-    <t xml:space="preserve">Använde: </t>
-  </si>
-  <si>
     <t>-          om API för login i backend är uppbyggd för att kunna hantera vidare påbyggnad för login i frontend</t>
   </si>
   <si>
@@ -494,9 +491,6 @@
     <t>HTTP 200 + JSON-array med objekt</t>
   </si>
   <si>
-    <t>Skickar null-värden om kolumnen i databasen saknar värde eller inte är med i querien, exempel case_handler vid unopened och chatToken</t>
-  </si>
-  <si>
     <t>2025-04-09</t>
   </si>
   <si>
@@ -575,9 +569,6 @@
     <t>Partly success / Bug</t>
   </si>
   <si>
-    <t>2025-04-10</t>
-  </si>
-  <si>
     <t>HTTP 200 + JSON-object med rätt struktur: caseDetails, messages (array med meddelanden) och user.</t>
   </si>
   <si>
@@ -587,17 +578,111 @@
     <t>Onödigt mycket data skickas till frontend, vilket också gör API requesten osäker, bl.a. för att både id och chatToken skickas med. I readern i backend  borde endast följande skickas för caseDetails: title, customer_fist_name, customer_last_name och messages: text, timestamp samt is_sender_customer. DTO</t>
   </si>
   <si>
-    <t>- Inga restriktioner finns på API-endpoints eftersom autentisering saknas i projektet.
+    <t>HTTP 200 + JSON-object med messages och user</t>
+  </si>
+  <si>
+    <t>Hämtar endast meddelanden och handläggare. Frontend är byggd för att hämta ärendedata från redan hämtad data i annan komponent.</t>
+  </si>
+  <si>
+    <t>HTTP 201 + return object with new message</t>
+  </si>
+  <si>
+    <t>I grunden fungerar API väl, efterwsom det nya meddelandet skickas tillbaka till frontend i ett objekt, vilket ger möjlighet till att uppdatera frontend utan en refresh (hämta data via API igen). Däremot skickas också en url inkluderad med nytt id, vilket jag upplever som onödigt utifrån ett säkerhetsperspektiv.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HTTP 200 + sträng med meddelande om att ärende med id x har stängts. </t>
+  </si>
+  <si>
+    <t>Success / Bug</t>
+  </si>
+  <si>
+    <t>Felhanteringen i API fungerar inte. Dels saknas det ett säkerställande i querien om att ärendet inte får vara stängt sedan innan (WHERE status != 'closed'). Logiken för att ta hand om ett ej befintligt ärende-id finns men inte för att ett ärende redan är stängt. Om samma ärende "stängs" skickas att det lyckade till frontend.</t>
+  </si>
+  <si>
+    <t>HTTP 404 när ingen är inloggad
+HTTP 200 + Användardata när någon är inloggad</t>
+  </si>
+  <si>
+    <t>Sucess</t>
+  </si>
+  <si>
+    <t>Hämtar session data om någon är inloggad och skickar felkod samt meddelande om att ingen är inloggad när så är.</t>
+  </si>
+  <si>
+    <t>HTTP 200</t>
+  </si>
+  <si>
+    <t>Sätter användare till session, men kollar inte om användaren är aktiv (slutat) eller inte. En medarbetare som har slutat kan alltså logga in, vilket skapar en säkerhetsbrist.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HTTP 200 / HTTP 400 </t>
+  </si>
+  <si>
+    <t>Loggar ut om inloggad med meddelande att användaren har blivit utloggad och ger 409 med meddelande att ingen är inloggad om ej så.</t>
+  </si>
+  <si>
+    <t>Hämtar alla användare i en array men skickar med all data om en användare inklusive password, vilket skapar en säkerhetsbrist. Heller ingen restriktion om vem som kan hämta alla användare.</t>
+  </si>
+  <si>
+    <t>Sucess / Refactor</t>
+  </si>
+  <si>
+    <t>Skulle behöva en DTO som avgör hur mycket data som skickas till frontend. All data skickas nu. Det görs heller inget urval  om ett ärende är öppet eller inte. Stängda ärenden borde skickas via en egen API, Eftersom listan för varje medarbetare borde visa aktiva ärenden endast.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- Inga restriktioner finns på API-endpoints eftersom autentisering saknas i projektet.
 - Namngivningskonventioner: 
 --Exempel: chatToken (korrekt C#), case_handler (inkorrekt C#) - Class Case.'Generell kommentar'!
 - Ingen hantering för att en kundtjänstmedarbetare ska kunna ta ett ärende, varken i backend eller frontend. Kan endast hårdkodas i databasen i dagsläget
-- Skalbarhet - Enum för category och status gör att skalbarheten till andra typer av företag begränsas. Dessa skulle behöva göras om till strängar och som kan sättas av admin i frontend.</t>
-  </si>
-  <si>
-    <t>HTTP 200 + JSON-object med messages och user</t>
-  </si>
-  <si>
-    <t>Hämtar endast meddelanden och handläggare. Frontend är byggd för att hämta ärendedata från redan hämtad data i annan komponent.</t>
+- Skalbarhet - Enum för category och status gör att skalbarheten till andra typer av företag begränsas. Dessa skulle behöva göras om till strängar och som kan sättas av admin i frontend.
+- API uppbyggda på olika sätt. Några returnerar ett object (nytt chattmeddelande), några fel id (nytt kundärende skickar meddelande-id istället för ärende-id).
+- Eftersom session inte finns implementerad har hanteringen av kund/kundtjänstmeddelande hanterats genom databasen: is_sender_customer, vilket avgör hur chatten beter sig i frontend. Borde varit gjort genom att frontend läser av session.
+- Tänkt lite fel. Session är implementerad i backend. Det är bara i frontend som den inte hanteras.
+- Detaljer i förhållande till säkerhet saknas i många fall: Exempel: inaktiv medarbetare kan logga in, skickar data till frontend som inte behövs (bla i ärendehantering), 
+- Inga restriktioner på API i förhållande till inloggad användare i session
+- Lärdom: Att kritiskt granska och testa API så ser man hur man skulle kunna bygga upp en endpoint bättre, både genom vilken data som hämtas, returneras  och hur säkerheten ska hanteras exempelvis genom att låsa api till session och användare. </t>
+  </si>
+  <si>
+    <t>HTTP 201</t>
+  </si>
+  <si>
+    <t>Sucess / Refactor / Restrict</t>
+  </si>
+  <si>
+    <t>Användare skapas men returnerar ett objekt med all insatt data, inklusive lösenord. Bättre hade varit att ha ett objekt som returnerar success tillsammans med id, user_name, ev mejladress.</t>
+  </si>
+  <si>
+    <t>HTTP 200 + Uppdaterad beroende på vad som uppdateras.</t>
+  </si>
+  <si>
+    <t>2024-04-09</t>
+  </si>
+  <si>
+    <t>Uppdaterar användare dynamiskt, att man alltså kan lägga till vilka värden som man vill ska uppdateras och utelämna andra. Däremot finns det ingen restriktion på att uppdatera vad som helst på användaren, så lösenord kan ändras utan problem. Om du däremot inte skickar med Active = true, ändras Active till false.</t>
+  </si>
+  <si>
+    <t>HTTP 500. Ska inte kunna gå att ta bort en användare, eftersom FK till cases</t>
+  </si>
+  <si>
+    <t>Onödig API för det ska inte gå att ta bort en användare från databasen. De ska kunna sättas inaktiva eller tas bort genom soft delete från frontend.</t>
+  </si>
+  <si>
+    <t>HTTP 200 + meddelande om ok</t>
+  </si>
+  <si>
+    <t>En användares möjlighet till att skapa ett eget lösenord fungerar, men eftersom databasen inte har unique på användare kan två användare med samma användarnamn uppdateras samtidigt men detta syns inte i responsen eftersom  samma meddelande skickas oavsett hur många rader som påverkas.</t>
+  </si>
+  <si>
+    <t>Skickar null-värden om kolumnen i databasen saknar värde eller inte är med i querien, exempel case_handler vid unopened och chatToken. Skickar för mycket data.</t>
+  </si>
+  <si>
+    <t>Success / Refactor / Restrict</t>
+  </si>
+  <si>
+    <t>Success /  Refactor / Restrict</t>
+  </si>
+  <si>
+    <t>Asmycket problem för att få tag i element pga MUI och inte varit noga med naming av element.</t>
   </si>
 </sst>
 </file>
@@ -2156,7 +2241,7 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A18" s="10" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
@@ -2397,7 +2482,7 @@
     </row>
     <row r="2" spans="1:7" ht="22" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
@@ -3504,8 +3589,8 @@
   <dimension ref="A1:I39"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F17" sqref="F17"/>
+      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E32" sqref="E32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3602,7 +3687,7 @@
         <v>119</v>
       </c>
       <c r="D4" s="12" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="E4" s="12"/>
       <c r="F4" s="12" t="s">
@@ -3623,7 +3708,7 @@
         <v>120</v>
       </c>
       <c r="D5" s="12" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="E5" s="12"/>
       <c r="F5" s="12"/>
@@ -3714,24 +3799,24 @@
         <v>85</v>
       </c>
       <c r="B12" s="12" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="C12" s="12" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="D12" s="12" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="E12" s="12" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="F12" s="12"/>
       <c r="G12" s="12"/>
       <c r="H12" s="12" t="s">
-        <v>149</v>
+        <v>179</v>
       </c>
       <c r="I12" s="12" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
     </row>
     <row r="13" spans="1:9" s="4" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
@@ -3745,20 +3830,20 @@
         <v>120</v>
       </c>
       <c r="D13" s="12" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="E13" s="12"/>
       <c r="F13" s="12" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="G13" s="12" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="H13" s="12" t="s">
-        <v>149</v>
+        <v>179</v>
       </c>
       <c r="I13" s="12" t="s">
-        <v>153</v>
+        <v>209</v>
       </c>
     </row>
     <row r="14" spans="1:9" s="4" customFormat="1" ht="42" x14ac:dyDescent="0.25">
@@ -3772,22 +3857,22 @@
         <v>120</v>
       </c>
       <c r="D14" s="12" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="E14" s="12" t="s">
         <v>115</v>
       </c>
       <c r="F14" s="12" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="G14" s="12" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="H14" s="12" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="I14" s="12" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="15" spans="1:9" s="4" customFormat="1" ht="52.5" x14ac:dyDescent="0.25">
@@ -3801,25 +3886,25 @@
         <v>121</v>
       </c>
       <c r="D15" s="12" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="E15" s="12" t="s">
+        <v>176</v>
+      </c>
+      <c r="F15" s="12" t="s">
         <v>178</v>
       </c>
-      <c r="F15" s="12" t="s">
-        <v>181</v>
-      </c>
       <c r="G15" s="12" t="s">
+        <v>150</v>
+      </c>
+      <c r="H15" s="12" t="s">
+        <v>211</v>
+      </c>
+      <c r="I15" s="12" t="s">
         <v>180</v>
       </c>
-      <c r="H15" s="12" t="s">
-        <v>182</v>
-      </c>
-      <c r="I15" s="12" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" s="4" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="1:9" s="4" customFormat="1" ht="52.5" x14ac:dyDescent="0.25">
       <c r="A16" s="12" t="s">
         <v>89</v>
       </c>
@@ -3830,15 +3915,23 @@
         <v>121</v>
       </c>
       <c r="D16" s="12" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="E16" s="12"/>
-      <c r="F16" s="12"/>
-      <c r="G16" s="12"/>
-      <c r="H16" s="12"/>
-      <c r="I16" s="12"/>
-    </row>
-    <row r="17" spans="1:9" s="4" customFormat="1" ht="42" x14ac:dyDescent="0.25">
+      <c r="F16" s="12" t="s">
+        <v>183</v>
+      </c>
+      <c r="G16" s="12" t="s">
+        <v>152</v>
+      </c>
+      <c r="H16" s="12" t="s">
+        <v>179</v>
+      </c>
+      <c r="I16" s="12" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" s="4" customFormat="1" ht="52.5" x14ac:dyDescent="0.25">
       <c r="A17" s="12" t="s">
         <v>90</v>
       </c>
@@ -3849,20 +3942,20 @@
         <v>121</v>
       </c>
       <c r="D17" s="12" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="E17" s="12"/>
       <c r="F17" s="12" t="s">
         <v>185</v>
       </c>
       <c r="G17" s="12" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="H17" s="12" t="s">
-        <v>149</v>
+        <v>186</v>
       </c>
       <c r="I17" s="12" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
     </row>
     <row r="18" spans="1:9" s="4" customFormat="1" ht="42" x14ac:dyDescent="0.25">
@@ -3876,13 +3969,21 @@
         <v>121</v>
       </c>
       <c r="D18" s="12" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="E18" s="12"/>
-      <c r="F18" s="12"/>
-      <c r="G18" s="12"/>
-      <c r="H18" s="12"/>
-      <c r="I18" s="12"/>
+      <c r="F18" s="12" t="s">
+        <v>181</v>
+      </c>
+      <c r="G18" s="12" t="s">
+        <v>150</v>
+      </c>
+      <c r="H18" s="12" t="s">
+        <v>148</v>
+      </c>
+      <c r="I18" s="12" t="s">
+        <v>182</v>
+      </c>
     </row>
     <row r="19" spans="1:9" s="4" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A19" s="12" t="s">
@@ -3895,15 +3996,23 @@
         <v>122</v>
       </c>
       <c r="D19" s="12" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="E19" s="12" t="s">
-        <v>147</v>
-      </c>
-      <c r="F19" s="12"/>
-      <c r="G19" s="12"/>
-      <c r="H19" s="12"/>
-      <c r="I19" s="12"/>
+        <v>146</v>
+      </c>
+      <c r="F19" s="12" t="s">
+        <v>188</v>
+      </c>
+      <c r="G19" s="12" t="s">
+        <v>150</v>
+      </c>
+      <c r="H19" s="12" t="s">
+        <v>189</v>
+      </c>
+      <c r="I19" s="12" t="s">
+        <v>190</v>
+      </c>
     </row>
     <row r="20" spans="1:9" s="4" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A20" s="12" t="s">
@@ -3916,15 +4025,23 @@
         <v>122</v>
       </c>
       <c r="D20" s="12" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="E20" s="12" t="s">
-        <v>147</v>
-      </c>
-      <c r="F20" s="12"/>
-      <c r="G20" s="12"/>
-      <c r="H20" s="12"/>
-      <c r="I20" s="12"/>
+        <v>146</v>
+      </c>
+      <c r="F20" s="12" t="s">
+        <v>193</v>
+      </c>
+      <c r="G20" s="12" t="s">
+        <v>152</v>
+      </c>
+      <c r="H20" s="12" t="s">
+        <v>210</v>
+      </c>
+      <c r="I20" s="12" t="s">
+        <v>192</v>
+      </c>
     </row>
     <row r="21" spans="1:9" s="4" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A21" s="12" t="s">
@@ -3937,15 +4054,23 @@
         <v>122</v>
       </c>
       <c r="D21" s="12" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="E21" s="12" t="s">
-        <v>147</v>
-      </c>
-      <c r="F21" s="12"/>
-      <c r="G21" s="12"/>
-      <c r="H21" s="12"/>
-      <c r="I21" s="12"/>
+        <v>146</v>
+      </c>
+      <c r="F21" s="12" t="s">
+        <v>193</v>
+      </c>
+      <c r="G21" s="12" t="s">
+        <v>152</v>
+      </c>
+      <c r="H21" s="12" t="s">
+        <v>148</v>
+      </c>
+      <c r="I21" s="12" t="s">
+        <v>194</v>
+      </c>
     </row>
     <row r="22" spans="1:9" s="4" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A22" s="12" t="s">
@@ -3958,15 +4083,23 @@
         <v>124</v>
       </c>
       <c r="D22" s="12" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="E22" s="12"/>
-      <c r="F22" s="12"/>
-      <c r="G22" s="12"/>
-      <c r="H22" s="12"/>
-      <c r="I22" s="12"/>
-    </row>
-    <row r="23" spans="1:9" s="4" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="F22" s="12" t="s">
+        <v>191</v>
+      </c>
+      <c r="G22" s="12" t="s">
+        <v>152</v>
+      </c>
+      <c r="H22" s="12" t="s">
+        <v>210</v>
+      </c>
+      <c r="I22" s="12" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" s="4" customFormat="1" ht="52.5" x14ac:dyDescent="0.25">
       <c r="A23" s="12" t="s">
         <v>96</v>
       </c>
@@ -3977,15 +4110,23 @@
         <v>124</v>
       </c>
       <c r="D23" s="12" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="E23" s="12" t="s">
         <v>125</v>
       </c>
-      <c r="F23" s="12"/>
-      <c r="G23" s="12"/>
-      <c r="H23" s="12"/>
-      <c r="I23" s="12"/>
+      <c r="F23" s="12" t="s">
+        <v>191</v>
+      </c>
+      <c r="G23" s="12" t="s">
+        <v>152</v>
+      </c>
+      <c r="H23" s="12" t="s">
+        <v>196</v>
+      </c>
+      <c r="I23" s="12" t="s">
+        <v>197</v>
+      </c>
     </row>
     <row r="24" spans="1:9" s="4" customFormat="1" ht="42" x14ac:dyDescent="0.25">
       <c r="A24" s="12" t="s">
@@ -3998,15 +4139,23 @@
         <v>124</v>
       </c>
       <c r="D24" s="12" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="E24" s="12"/>
-      <c r="F24" s="12"/>
-      <c r="G24" s="12"/>
-      <c r="H24" s="12"/>
-      <c r="I24" s="12"/>
-    </row>
-    <row r="25" spans="1:9" s="4" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="F24" s="12" t="s">
+        <v>199</v>
+      </c>
+      <c r="G24" s="12" t="s">
+        <v>152</v>
+      </c>
+      <c r="H24" s="12" t="s">
+        <v>200</v>
+      </c>
+      <c r="I24" s="12" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" s="4" customFormat="1" ht="52.5" x14ac:dyDescent="0.25">
       <c r="A25" s="12" t="s">
         <v>98</v>
       </c>
@@ -4017,15 +4166,23 @@
         <v>124</v>
       </c>
       <c r="D25" s="12" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="E25" s="12" t="s">
         <v>126</v>
       </c>
-      <c r="F25" s="12"/>
-      <c r="G25" s="12"/>
-      <c r="H25" s="12"/>
-      <c r="I25" s="12"/>
+      <c r="F25" s="12" t="s">
+        <v>202</v>
+      </c>
+      <c r="G25" s="12" t="s">
+        <v>203</v>
+      </c>
+      <c r="H25" s="12" t="s">
+        <v>200</v>
+      </c>
+      <c r="I25" s="12" t="s">
+        <v>204</v>
+      </c>
     </row>
     <row r="26" spans="1:9" s="4" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A26" s="12" t="s">
@@ -4038,17 +4195,25 @@
         <v>124</v>
       </c>
       <c r="D26" s="12" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="E26" s="12" t="s">
         <v>127</v>
       </c>
-      <c r="F26" s="12"/>
-      <c r="G26" s="12"/>
-      <c r="H26" s="12"/>
-      <c r="I26" s="12"/>
-    </row>
-    <row r="27" spans="1:9" s="4" customFormat="1" ht="42" x14ac:dyDescent="0.25">
+      <c r="F26" s="12" t="s">
+        <v>205</v>
+      </c>
+      <c r="G26" s="12" t="s">
+        <v>203</v>
+      </c>
+      <c r="H26" s="12" t="s">
+        <v>148</v>
+      </c>
+      <c r="I26" s="12" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" s="4" customFormat="1" ht="52.5" x14ac:dyDescent="0.25">
       <c r="A27" s="12" t="s">
         <v>100</v>
       </c>
@@ -4059,13 +4224,21 @@
         <v>124</v>
       </c>
       <c r="D27" s="12" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="E27" s="12"/>
-      <c r="F27" s="12"/>
-      <c r="G27" s="12"/>
-      <c r="H27" s="12"/>
-      <c r="I27" s="12"/>
+      <c r="F27" s="12" t="s">
+        <v>207</v>
+      </c>
+      <c r="G27" s="12" t="s">
+        <v>203</v>
+      </c>
+      <c r="H27" s="12" t="s">
+        <v>210</v>
+      </c>
+      <c r="I27" s="12" t="s">
+        <v>208</v>
+      </c>
     </row>
     <row r="28" spans="1:9" s="4" customFormat="1" ht="21" x14ac:dyDescent="0.25">
       <c r="A28" s="12" t="s">
@@ -4085,7 +4258,7 @@
       <c r="G28" s="12"/>
       <c r="H28" s="12"/>
       <c r="I28" s="12" t="s">
-        <v>144</v>
+        <v>212</v>
       </c>
     </row>
     <row r="29" spans="1:9" s="4" customFormat="1" ht="21" x14ac:dyDescent="0.25">
@@ -4258,7 +4431,7 @@
       <c r="H38" s="12"/>
       <c r="I38" s="12"/>
     </row>
-    <row r="39" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:9" s="4" customFormat="1" ht="10.5" x14ac:dyDescent="0.25">
       <c r="A39" s="12" t="s">
         <v>112</v>
       </c>
@@ -4295,12 +4468,12 @@
   <sheetData>
     <row r="1" spans="1:1" ht="64" x14ac:dyDescent="0.35">
       <c r="A1" s="11" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A2" s="14" t="s">
-        <v>184</v>
+        <v>198</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
test(UI): added test cases 027 and 028 testing NewCustomerCase
</commit_message>
<xml_diff>
--- a/Documentation/Testplanering_Testfall.xlsx
+++ b/Documentation/Testplanering_Testfall.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Local\Peter\Testning\SecuremeTesting@fendraq\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BFCE26F-7AED-4C6E-BB58-741890DF2A95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF2872D0-8BF8-4390-AD6E-49DDDBA94B7D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" firstSheet="2" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="213">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="292" uniqueCount="220">
   <si>
     <t>Test-ID</t>
   </si>
@@ -462,9 +462,6 @@
   </si>
   <si>
     <t>EX: Testar med både null och giltig input</t>
-  </si>
-  <si>
-    <t>Fälten validerar korrekt input och visar felmeddelanden</t>
   </si>
   <si>
     <t>-          om API för login i backend är uppbyggd för att kunna hantera vidare påbyggnad för login i frontend</t>
@@ -682,7 +679,31 @@
     <t>Success /  Refactor / Restrict</t>
   </si>
   <si>
-    <t>Asmycket problem för att få tag i element pga MUI och inte varit noga med naming av element.</t>
+    <t>TC-039</t>
+  </si>
+  <si>
+    <t>Verifiera att kundformuläret hanterar felaktig mejladress</t>
+  </si>
+  <si>
+    <t>TC-040</t>
+  </si>
+  <si>
+    <t>Verfiera att kundformuläret kräver fullständig information från kunden</t>
+  </si>
+  <si>
+    <t>Ett nytt ärende skapas och en alert med "Message sent successfully" visas.</t>
+  </si>
+  <si>
+    <t>Ett nytt ärende skapas inte och ett felmedelande genereras</t>
+  </si>
+  <si>
+    <t>2024-04-10</t>
+  </si>
+  <si>
+    <t>Bug</t>
+  </si>
+  <si>
+    <t>Det ligger inga restriktioner om att inputdata måste vara i ett visst format i frontend. Däremot skickar backend meddelande om att mejl inte kunde skickas</t>
   </si>
 </sst>
 </file>
@@ -2241,7 +2262,7 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A18" s="10" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
@@ -2482,7 +2503,7 @@
     </row>
     <row r="2" spans="1:7" ht="22" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
@@ -3586,11 +3607,11 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I39"/>
+  <dimension ref="A1:I41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E32" sqref="E32"/>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A27" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E30" sqref="E30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3687,7 +3708,7 @@
         <v>119</v>
       </c>
       <c r="D4" s="12" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E4" s="12"/>
       <c r="F4" s="12" t="s">
@@ -3708,7 +3729,7 @@
         <v>120</v>
       </c>
       <c r="D5" s="12" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="E5" s="12"/>
       <c r="F5" s="12"/>
@@ -3799,24 +3820,24 @@
         <v>85</v>
       </c>
       <c r="B12" s="12" t="s">
+        <v>153</v>
+      </c>
+      <c r="C12" s="12" t="s">
         <v>154</v>
       </c>
-      <c r="C12" s="12" t="s">
-        <v>155</v>
-      </c>
       <c r="D12" s="12" t="s">
+        <v>172</v>
+      </c>
+      <c r="E12" s="12" t="s">
         <v>173</v>
-      </c>
-      <c r="E12" s="12" t="s">
-        <v>174</v>
       </c>
       <c r="F12" s="12"/>
       <c r="G12" s="12"/>
       <c r="H12" s="12" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="I12" s="12" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="13" spans="1:9" s="4" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
@@ -3830,20 +3851,20 @@
         <v>120</v>
       </c>
       <c r="D13" s="12" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="E13" s="12"/>
       <c r="F13" s="12" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="G13" s="12" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="H13" s="12" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="I13" s="12" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="14" spans="1:9" s="4" customFormat="1" ht="42" x14ac:dyDescent="0.25">
@@ -3857,22 +3878,22 @@
         <v>120</v>
       </c>
       <c r="D14" s="12" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="E14" s="12" t="s">
         <v>115</v>
       </c>
       <c r="F14" s="12" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="G14" s="12" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="H14" s="12" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="I14" s="12" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="15" spans="1:9" s="4" customFormat="1" ht="52.5" x14ac:dyDescent="0.25">
@@ -3886,22 +3907,22 @@
         <v>121</v>
       </c>
       <c r="D15" s="12" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="E15" s="12" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="F15" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="G15" s="12" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="H15" s="12" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="I15" s="12" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="16" spans="1:9" s="4" customFormat="1" ht="52.5" x14ac:dyDescent="0.25">
@@ -3915,20 +3936,20 @@
         <v>121</v>
       </c>
       <c r="D16" s="12" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="E16" s="12"/>
       <c r="F16" s="12" t="s">
+        <v>182</v>
+      </c>
+      <c r="G16" s="12" t="s">
+        <v>151</v>
+      </c>
+      <c r="H16" s="12" t="s">
+        <v>178</v>
+      </c>
+      <c r="I16" s="12" t="s">
         <v>183</v>
-      </c>
-      <c r="G16" s="12" t="s">
-        <v>152</v>
-      </c>
-      <c r="H16" s="12" t="s">
-        <v>179</v>
-      </c>
-      <c r="I16" s="12" t="s">
-        <v>184</v>
       </c>
     </row>
     <row r="17" spans="1:9" s="4" customFormat="1" ht="52.5" x14ac:dyDescent="0.25">
@@ -3942,20 +3963,20 @@
         <v>121</v>
       </c>
       <c r="D17" s="12" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="E17" s="12"/>
       <c r="F17" s="12" t="s">
+        <v>184</v>
+      </c>
+      <c r="G17" s="12" t="s">
+        <v>151</v>
+      </c>
+      <c r="H17" s="12" t="s">
         <v>185</v>
       </c>
-      <c r="G17" s="12" t="s">
-        <v>152</v>
-      </c>
-      <c r="H17" s="12" t="s">
+      <c r="I17" s="12" t="s">
         <v>186</v>
-      </c>
-      <c r="I17" s="12" t="s">
-        <v>187</v>
       </c>
     </row>
     <row r="18" spans="1:9" s="4" customFormat="1" ht="42" x14ac:dyDescent="0.25">
@@ -3969,20 +3990,20 @@
         <v>121</v>
       </c>
       <c r="D18" s="12" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E18" s="12"/>
       <c r="F18" s="12" t="s">
+        <v>180</v>
+      </c>
+      <c r="G18" s="12" t="s">
+        <v>149</v>
+      </c>
+      <c r="H18" s="12" t="s">
+        <v>147</v>
+      </c>
+      <c r="I18" s="12" t="s">
         <v>181</v>
-      </c>
-      <c r="G18" s="12" t="s">
-        <v>150</v>
-      </c>
-      <c r="H18" s="12" t="s">
-        <v>148</v>
-      </c>
-      <c r="I18" s="12" t="s">
-        <v>182</v>
       </c>
     </row>
     <row r="19" spans="1:9" s="4" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
@@ -3996,22 +4017,22 @@
         <v>122</v>
       </c>
       <c r="D19" s="12" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E19" s="12" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="F19" s="12" t="s">
+        <v>187</v>
+      </c>
+      <c r="G19" s="12" t="s">
+        <v>149</v>
+      </c>
+      <c r="H19" s="12" t="s">
         <v>188</v>
       </c>
-      <c r="G19" s="12" t="s">
-        <v>150</v>
-      </c>
-      <c r="H19" s="12" t="s">
+      <c r="I19" s="12" t="s">
         <v>189</v>
-      </c>
-      <c r="I19" s="12" t="s">
-        <v>190</v>
       </c>
     </row>
     <row r="20" spans="1:9" s="4" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
@@ -4025,22 +4046,22 @@
         <v>122</v>
       </c>
       <c r="D20" s="12" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E20" s="12" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="F20" s="12" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="G20" s="12" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="H20" s="12" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="I20" s="12" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="21" spans="1:9" s="4" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
@@ -4054,22 +4075,22 @@
         <v>122</v>
       </c>
       <c r="D21" s="12" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E21" s="12" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="F21" s="12" t="s">
+        <v>192</v>
+      </c>
+      <c r="G21" s="12" t="s">
+        <v>151</v>
+      </c>
+      <c r="H21" s="12" t="s">
+        <v>147</v>
+      </c>
+      <c r="I21" s="12" t="s">
         <v>193</v>
-      </c>
-      <c r="G21" s="12" t="s">
-        <v>152</v>
-      </c>
-      <c r="H21" s="12" t="s">
-        <v>148</v>
-      </c>
-      <c r="I21" s="12" t="s">
-        <v>194</v>
       </c>
     </row>
     <row r="22" spans="1:9" s="4" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
@@ -4083,20 +4104,20 @@
         <v>124</v>
       </c>
       <c r="D22" s="12" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="E22" s="12"/>
       <c r="F22" s="12" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="G22" s="12" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="H22" s="12" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="I22" s="12" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="23" spans="1:9" s="4" customFormat="1" ht="52.5" x14ac:dyDescent="0.25">
@@ -4110,22 +4131,22 @@
         <v>124</v>
       </c>
       <c r="D23" s="12" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="E23" s="12" t="s">
         <v>125</v>
       </c>
       <c r="F23" s="12" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="G23" s="12" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="H23" s="12" t="s">
+        <v>195</v>
+      </c>
+      <c r="I23" s="12" t="s">
         <v>196</v>
-      </c>
-      <c r="I23" s="12" t="s">
-        <v>197</v>
       </c>
     </row>
     <row r="24" spans="1:9" s="4" customFormat="1" ht="42" x14ac:dyDescent="0.25">
@@ -4139,20 +4160,20 @@
         <v>124</v>
       </c>
       <c r="D24" s="12" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="E24" s="12"/>
       <c r="F24" s="12" t="s">
+        <v>198</v>
+      </c>
+      <c r="G24" s="12" t="s">
+        <v>151</v>
+      </c>
+      <c r="H24" s="12" t="s">
         <v>199</v>
       </c>
-      <c r="G24" s="12" t="s">
-        <v>152</v>
-      </c>
-      <c r="H24" s="12" t="s">
+      <c r="I24" s="12" t="s">
         <v>200</v>
-      </c>
-      <c r="I24" s="12" t="s">
-        <v>201</v>
       </c>
     </row>
     <row r="25" spans="1:9" s="4" customFormat="1" ht="52.5" x14ac:dyDescent="0.25">
@@ -4166,22 +4187,22 @@
         <v>124</v>
       </c>
       <c r="D25" s="12" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="E25" s="12" t="s">
         <v>126</v>
       </c>
       <c r="F25" s="12" t="s">
+        <v>201</v>
+      </c>
+      <c r="G25" s="12" t="s">
         <v>202</v>
       </c>
-      <c r="G25" s="12" t="s">
+      <c r="H25" s="12" t="s">
+        <v>199</v>
+      </c>
+      <c r="I25" s="12" t="s">
         <v>203</v>
-      </c>
-      <c r="H25" s="12" t="s">
-        <v>200</v>
-      </c>
-      <c r="I25" s="12" t="s">
-        <v>204</v>
       </c>
     </row>
     <row r="26" spans="1:9" s="4" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
@@ -4195,22 +4216,22 @@
         <v>124</v>
       </c>
       <c r="D26" s="12" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E26" s="12" t="s">
         <v>127</v>
       </c>
       <c r="F26" s="12" t="s">
+        <v>204</v>
+      </c>
+      <c r="G26" s="12" t="s">
+        <v>202</v>
+      </c>
+      <c r="H26" s="12" t="s">
+        <v>147</v>
+      </c>
+      <c r="I26" s="12" t="s">
         <v>205</v>
-      </c>
-      <c r="G26" s="12" t="s">
-        <v>203</v>
-      </c>
-      <c r="H26" s="12" t="s">
-        <v>148</v>
-      </c>
-      <c r="I26" s="12" t="s">
-        <v>206</v>
       </c>
     </row>
     <row r="27" spans="1:9" s="4" customFormat="1" ht="52.5" x14ac:dyDescent="0.25">
@@ -4224,20 +4245,20 @@
         <v>124</v>
       </c>
       <c r="D27" s="12" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="E27" s="12"/>
       <c r="F27" s="12" t="s">
+        <v>206</v>
+      </c>
+      <c r="G27" s="12" t="s">
+        <v>202</v>
+      </c>
+      <c r="H27" s="12" t="s">
+        <v>209</v>
+      </c>
+      <c r="I27" s="12" t="s">
         <v>207</v>
-      </c>
-      <c r="G27" s="12" t="s">
-        <v>203</v>
-      </c>
-      <c r="H27" s="12" t="s">
-        <v>210</v>
-      </c>
-      <c r="I27" s="12" t="s">
-        <v>208</v>
       </c>
     </row>
     <row r="28" spans="1:9" s="4" customFormat="1" ht="21" x14ac:dyDescent="0.25">
@@ -4253,15 +4274,17 @@
       </c>
       <c r="E28" s="12"/>
       <c r="F28" s="12" t="s">
-        <v>143</v>
-      </c>
-      <c r="G28" s="12"/>
-      <c r="H28" s="12"/>
-      <c r="I28" s="12" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" s="4" customFormat="1" ht="21" x14ac:dyDescent="0.25">
+        <v>215</v>
+      </c>
+      <c r="G28" s="12" t="s">
+        <v>217</v>
+      </c>
+      <c r="H28" s="12" t="s">
+        <v>147</v>
+      </c>
+      <c r="I28" s="12"/>
+    </row>
+    <row r="29" spans="1:9" s="4" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A29" s="12" t="s">
         <v>102</v>
       </c>
@@ -4270,13 +4293,21 @@
       </c>
       <c r="C29" s="12"/>
       <c r="D29" s="12" t="s">
-        <v>131</v>
+        <v>212</v>
       </c>
       <c r="E29" s="12"/>
-      <c r="F29" s="12"/>
-      <c r="G29" s="12"/>
-      <c r="H29" s="12"/>
-      <c r="I29" s="12"/>
+      <c r="F29" s="12" t="s">
+        <v>216</v>
+      </c>
+      <c r="G29" s="12" t="s">
+        <v>217</v>
+      </c>
+      <c r="H29" s="12" t="s">
+        <v>218</v>
+      </c>
+      <c r="I29" s="12" t="s">
+        <v>219</v>
+      </c>
     </row>
     <row r="30" spans="1:9" s="4" customFormat="1" ht="21" x14ac:dyDescent="0.25">
       <c r="A30" s="12" t="s">
@@ -4287,11 +4318,9 @@
       </c>
       <c r="C30" s="12"/>
       <c r="D30" s="12" t="s">
-        <v>132</v>
-      </c>
-      <c r="E30" s="12" t="s">
-        <v>135</v>
-      </c>
+        <v>214</v>
+      </c>
+      <c r="E30" s="12"/>
       <c r="F30" s="12"/>
       <c r="G30" s="12"/>
       <c r="H30" s="12"/>
@@ -4306,11 +4335,9 @@
       </c>
       <c r="C31" s="12"/>
       <c r="D31" s="12" t="s">
-        <v>133</v>
-      </c>
-      <c r="E31" s="12" t="s">
-        <v>135</v>
-      </c>
+        <v>131</v>
+      </c>
+      <c r="E31" s="12"/>
       <c r="F31" s="12"/>
       <c r="G31" s="12"/>
       <c r="H31" s="12"/>
@@ -4325,7 +4352,7 @@
       </c>
       <c r="C32" s="12"/>
       <c r="D32" s="12" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="E32" s="12" t="s">
         <v>135</v>
@@ -4344,15 +4371,17 @@
       </c>
       <c r="C33" s="12"/>
       <c r="D33" s="12" t="s">
-        <v>136</v>
-      </c>
-      <c r="E33" s="12"/>
+        <v>133</v>
+      </c>
+      <c r="E33" s="12" t="s">
+        <v>135</v>
+      </c>
       <c r="F33" s="12"/>
       <c r="G33" s="12"/>
       <c r="H33" s="12"/>
       <c r="I33" s="12"/>
     </row>
-    <row r="34" spans="1:9" s="4" customFormat="1" ht="10.5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:9" s="4" customFormat="1" ht="21" x14ac:dyDescent="0.25">
       <c r="A34" s="12" t="s">
         <v>107</v>
       </c>
@@ -4361,15 +4390,17 @@
       </c>
       <c r="C34" s="12"/>
       <c r="D34" s="12" t="s">
-        <v>137</v>
-      </c>
-      <c r="E34" s="12"/>
+        <v>134</v>
+      </c>
+      <c r="E34" s="12" t="s">
+        <v>135</v>
+      </c>
       <c r="F34" s="12"/>
       <c r="G34" s="12"/>
       <c r="H34" s="12"/>
       <c r="I34" s="12"/>
     </row>
-    <row r="35" spans="1:9" s="4" customFormat="1" ht="10.5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:9" s="4" customFormat="1" ht="21" x14ac:dyDescent="0.25">
       <c r="A35" s="12" t="s">
         <v>108</v>
       </c>
@@ -4378,7 +4409,7 @@
       </c>
       <c r="C35" s="12"/>
       <c r="D35" s="12" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="E35" s="12"/>
       <c r="F35" s="12"/>
@@ -4394,7 +4425,9 @@
         <v>129</v>
       </c>
       <c r="C36" s="12"/>
-      <c r="D36" s="12"/>
+      <c r="D36" s="12" t="s">
+        <v>137</v>
+      </c>
       <c r="E36" s="12"/>
       <c r="F36" s="12"/>
       <c r="G36" s="12"/>
@@ -4409,7 +4442,9 @@
         <v>129</v>
       </c>
       <c r="C37" s="12"/>
-      <c r="D37" s="12"/>
+      <c r="D37" s="12" t="s">
+        <v>138</v>
+      </c>
       <c r="E37" s="12"/>
       <c r="F37" s="12"/>
       <c r="G37" s="12"/>
@@ -4421,7 +4456,7 @@
         <v>111</v>
       </c>
       <c r="B38" s="12" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="C38" s="12"/>
       <c r="D38" s="12"/>
@@ -4436,7 +4471,7 @@
         <v>112</v>
       </c>
       <c r="B39" s="12" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="C39" s="12"/>
       <c r="D39" s="12"/>
@@ -4445,6 +4480,36 @@
       <c r="G39" s="12"/>
       <c r="H39" s="12"/>
       <c r="I39" s="12"/>
+    </row>
+    <row r="40" spans="1:9" s="4" customFormat="1" ht="10.5" x14ac:dyDescent="0.25">
+      <c r="A40" s="12" t="s">
+        <v>211</v>
+      </c>
+      <c r="B40" s="12" t="s">
+        <v>128</v>
+      </c>
+      <c r="C40" s="12"/>
+      <c r="D40" s="12"/>
+      <c r="E40" s="12"/>
+      <c r="F40" s="12"/>
+      <c r="G40" s="12"/>
+      <c r="H40" s="12"/>
+      <c r="I40" s="12"/>
+    </row>
+    <row r="41" spans="1:9" s="4" customFormat="1" ht="10.5" x14ac:dyDescent="0.25">
+      <c r="A41" s="12" t="s">
+        <v>213</v>
+      </c>
+      <c r="B41" s="12" t="s">
+        <v>128</v>
+      </c>
+      <c r="C41" s="12"/>
+      <c r="D41" s="12"/>
+      <c r="E41" s="12"/>
+      <c r="F41" s="12"/>
+      <c r="G41" s="12"/>
+      <c r="H41" s="12"/>
+      <c r="I41" s="12"/>
     </row>
   </sheetData>
   <phoneticPr fontId="6" type="noConversion"/>
@@ -4468,12 +4533,12 @@
   <sheetData>
     <row r="1" spans="1:1" ht="64" x14ac:dyDescent="0.35">
       <c r="A1" s="11" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A2" s="14" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
test(UI) added test for chat as a customer
</commit_message>
<xml_diff>
--- a/Documentation/Testplanering_Testfall.xlsx
+++ b/Documentation/Testplanering_Testfall.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Local\Peter\Testning\SecuremeTesting@fendraq\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF2872D0-8BF8-4390-AD6E-49DDDBA94B7D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87BF5DAA-D02C-48C3-A817-2333FC07C92A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" firstSheet="2" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="292" uniqueCount="220">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="224">
   <si>
     <t>Test-ID</t>
   </si>
@@ -652,9 +652,6 @@
     <t>HTTP 200 + Uppdaterad beroende på vad som uppdateras.</t>
   </si>
   <si>
-    <t>2024-04-09</t>
-  </si>
-  <si>
     <t>Uppdaterar användare dynamiskt, att man alltså kan lägga till vilka värden som man vill ska uppdateras och utelämna andra. Däremot finns det ingen restriktion på att uppdatera vad som helst på användaren, så lösenord kan ändras utan problem. Om du däremot inte skickar med Active = true, ändras Active till false.</t>
   </si>
   <si>
@@ -697,13 +694,28 @@
     <t>Ett nytt ärende skapas inte och ett felmedelande genereras</t>
   </si>
   <si>
-    <t>2024-04-10</t>
-  </si>
-  <si>
     <t>Bug</t>
   </si>
   <si>
     <t>Det ligger inga restriktioner om att inputdata måste vara i ett visst format i frontend. Däremot skickar backend meddelande om att mejl inte kunde skickas</t>
+  </si>
+  <si>
+    <t>2025-04-11</t>
+  </si>
+  <si>
+    <t>Ett nytt ärende skapas inte och ett felmeddelande genereras som informerar att alla fält är obligatoriska</t>
+  </si>
+  <si>
+    <t>En unik chatt öppnas för kunden</t>
+  </si>
+  <si>
+    <t>Behövs fler assertions?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lade till klassnamn för att lättare nå elementen. Men chatten uppdaterar inte automatiskt. </t>
+  </si>
+  <si>
+    <t>Kunden kan skriva ett meddelande som visas när sidan uppdateras.</t>
   </si>
 </sst>
 </file>
@@ -857,7 +869,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1" readingOrder="1"/>
@@ -904,6 +916,18 @@
     </xf>
     <xf numFmtId="49" fontId="2" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3609,9 +3633,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I41"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A27" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E30" sqref="E30"/>
+      <selection pane="bottomLeft" activeCell="F33" sqref="F33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3620,7 +3644,8 @@
     <col min="2" max="3" width="11.1796875" style="13" customWidth="1"/>
     <col min="4" max="5" width="27.453125" style="13" customWidth="1"/>
     <col min="6" max="6" width="25.6328125" style="13" customWidth="1"/>
-    <col min="7" max="8" width="11.1796875" style="13" customWidth="1"/>
+    <col min="7" max="7" width="11.1796875" style="20" customWidth="1"/>
+    <col min="8" max="8" width="11.1796875" style="13" customWidth="1"/>
     <col min="9" max="9" width="42.26953125" style="13" customWidth="1"/>
   </cols>
   <sheetData>
@@ -3643,7 +3668,7 @@
       <c r="F1" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="11" t="s">
+      <c r="G1" s="18" t="s">
         <v>3</v>
       </c>
       <c r="H1" s="11" t="s">
@@ -3670,7 +3695,7 @@
       <c r="F2" s="12" t="s">
         <v>141</v>
       </c>
-      <c r="G2" s="12"/>
+      <c r="G2" s="17"/>
       <c r="H2" s="12"/>
       <c r="I2" s="12" t="s">
         <v>142</v>
@@ -3693,7 +3718,7 @@
       <c r="F3" s="12" t="s">
         <v>141</v>
       </c>
-      <c r="G3" s="12"/>
+      <c r="G3" s="17"/>
       <c r="H3" s="12"/>
       <c r="I3" s="12"/>
     </row>
@@ -3714,7 +3739,7 @@
       <c r="F4" s="12" t="s">
         <v>141</v>
       </c>
-      <c r="G4" s="12"/>
+      <c r="G4" s="17"/>
       <c r="H4" s="12"/>
       <c r="I4" s="12"/>
     </row>
@@ -3733,7 +3758,7 @@
       </c>
       <c r="E5" s="12"/>
       <c r="F5" s="12"/>
-      <c r="G5" s="12"/>
+      <c r="G5" s="17"/>
       <c r="H5" s="12"/>
       <c r="I5" s="12"/>
     </row>
@@ -3746,7 +3771,7 @@
       <c r="D6" s="12"/>
       <c r="E6" s="12"/>
       <c r="F6" s="12"/>
-      <c r="G6" s="12"/>
+      <c r="G6" s="17"/>
       <c r="H6" s="12"/>
       <c r="I6" s="12"/>
     </row>
@@ -3759,7 +3784,7 @@
       <c r="D7" s="12"/>
       <c r="E7" s="12"/>
       <c r="F7" s="12"/>
-      <c r="G7" s="12"/>
+      <c r="G7" s="17"/>
       <c r="H7" s="12"/>
       <c r="I7" s="12"/>
     </row>
@@ -3772,7 +3797,7 @@
       <c r="D8" s="12"/>
       <c r="E8" s="12"/>
       <c r="F8" s="12"/>
-      <c r="G8" s="12"/>
+      <c r="G8" s="17"/>
       <c r="H8" s="12"/>
       <c r="I8" s="12"/>
     </row>
@@ -3785,7 +3810,7 @@
       <c r="D9" s="12"/>
       <c r="E9" s="12"/>
       <c r="F9" s="12"/>
-      <c r="G9" s="12"/>
+      <c r="G9" s="17"/>
       <c r="H9" s="12"/>
       <c r="I9" s="12"/>
     </row>
@@ -3798,7 +3823,7 @@
       <c r="D10" s="12"/>
       <c r="E10" s="12"/>
       <c r="F10" s="12"/>
-      <c r="G10" s="12"/>
+      <c r="G10" s="17"/>
       <c r="H10" s="12"/>
       <c r="I10" s="12"/>
     </row>
@@ -3811,7 +3836,7 @@
       <c r="D11" s="12"/>
       <c r="E11" s="12"/>
       <c r="F11" s="12"/>
-      <c r="G11" s="12"/>
+      <c r="G11" s="17"/>
       <c r="H11" s="12"/>
       <c r="I11" s="12"/>
     </row>
@@ -3832,7 +3857,7 @@
         <v>173</v>
       </c>
       <c r="F12" s="12"/>
-      <c r="G12" s="12"/>
+      <c r="G12" s="17"/>
       <c r="H12" s="12" t="s">
         <v>178</v>
       </c>
@@ -3857,14 +3882,14 @@
       <c r="F13" s="12" t="s">
         <v>150</v>
       </c>
-      <c r="G13" s="12" t="s">
+      <c r="G13" s="17" t="s">
         <v>149</v>
       </c>
       <c r="H13" s="12" t="s">
         <v>178</v>
       </c>
       <c r="I13" s="12" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="14" spans="1:9" s="4" customFormat="1" ht="42" x14ac:dyDescent="0.25">
@@ -3886,7 +3911,7 @@
       <c r="F14" s="12" t="s">
         <v>146</v>
       </c>
-      <c r="G14" s="12" t="s">
+      <c r="G14" s="17" t="s">
         <v>149</v>
       </c>
       <c r="H14" s="12" t="s">
@@ -3915,11 +3940,11 @@
       <c r="F15" s="12" t="s">
         <v>177</v>
       </c>
-      <c r="G15" s="12" t="s">
+      <c r="G15" s="17" t="s">
         <v>149</v>
       </c>
       <c r="H15" s="12" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="I15" s="12" t="s">
         <v>179</v>
@@ -3942,7 +3967,7 @@
       <c r="F16" s="12" t="s">
         <v>182</v>
       </c>
-      <c r="G16" s="12" t="s">
+      <c r="G16" s="17" t="s">
         <v>151</v>
       </c>
       <c r="H16" s="12" t="s">
@@ -3969,7 +3994,7 @@
       <c r="F17" s="12" t="s">
         <v>184</v>
       </c>
-      <c r="G17" s="12" t="s">
+      <c r="G17" s="17" t="s">
         <v>151</v>
       </c>
       <c r="H17" s="12" t="s">
@@ -3996,7 +4021,7 @@
       <c r="F18" s="12" t="s">
         <v>180</v>
       </c>
-      <c r="G18" s="12" t="s">
+      <c r="G18" s="17" t="s">
         <v>149</v>
       </c>
       <c r="H18" s="12" t="s">
@@ -4025,7 +4050,7 @@
       <c r="F19" s="12" t="s">
         <v>187</v>
       </c>
-      <c r="G19" s="12" t="s">
+      <c r="G19" s="17" t="s">
         <v>149</v>
       </c>
       <c r="H19" s="12" t="s">
@@ -4054,11 +4079,11 @@
       <c r="F20" s="12" t="s">
         <v>192</v>
       </c>
-      <c r="G20" s="12" t="s">
+      <c r="G20" s="17" t="s">
         <v>151</v>
       </c>
       <c r="H20" s="12" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="I20" s="12" t="s">
         <v>191</v>
@@ -4083,7 +4108,7 @@
       <c r="F21" s="12" t="s">
         <v>192</v>
       </c>
-      <c r="G21" s="12" t="s">
+      <c r="G21" s="17" t="s">
         <v>151</v>
       </c>
       <c r="H21" s="12" t="s">
@@ -4110,11 +4135,11 @@
       <c r="F22" s="12" t="s">
         <v>190</v>
       </c>
-      <c r="G22" s="12" t="s">
+      <c r="G22" s="17" t="s">
         <v>151</v>
       </c>
       <c r="H22" s="12" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="I22" s="12" t="s">
         <v>194</v>
@@ -4139,7 +4164,7 @@
       <c r="F23" s="12" t="s">
         <v>190</v>
       </c>
-      <c r="G23" s="12" t="s">
+      <c r="G23" s="17" t="s">
         <v>151</v>
       </c>
       <c r="H23" s="12" t="s">
@@ -4166,7 +4191,7 @@
       <c r="F24" s="12" t="s">
         <v>198</v>
       </c>
-      <c r="G24" s="12" t="s">
+      <c r="G24" s="17" t="s">
         <v>151</v>
       </c>
       <c r="H24" s="12" t="s">
@@ -4195,14 +4220,14 @@
       <c r="F25" s="12" t="s">
         <v>201</v>
       </c>
-      <c r="G25" s="12" t="s">
-        <v>202</v>
+      <c r="G25" s="19">
+        <v>45756</v>
       </c>
       <c r="H25" s="12" t="s">
         <v>199</v>
       </c>
       <c r="I25" s="12" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="26" spans="1:9" s="4" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
@@ -4222,16 +4247,16 @@
         <v>127</v>
       </c>
       <c r="F26" s="12" t="s">
-        <v>204</v>
-      </c>
-      <c r="G26" s="12" t="s">
-        <v>202</v>
+        <v>203</v>
+      </c>
+      <c r="G26" s="19">
+        <v>45756</v>
       </c>
       <c r="H26" s="12" t="s">
         <v>147</v>
       </c>
       <c r="I26" s="12" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="27" spans="1:9" s="4" customFormat="1" ht="52.5" x14ac:dyDescent="0.25">
@@ -4249,16 +4274,16 @@
       </c>
       <c r="E27" s="12"/>
       <c r="F27" s="12" t="s">
+        <v>205</v>
+      </c>
+      <c r="G27" s="19">
+        <v>45756</v>
+      </c>
+      <c r="H27" s="12" t="s">
+        <v>208</v>
+      </c>
+      <c r="I27" s="12" t="s">
         <v>206</v>
-      </c>
-      <c r="G27" s="12" t="s">
-        <v>202</v>
-      </c>
-      <c r="H27" s="12" t="s">
-        <v>209</v>
-      </c>
-      <c r="I27" s="12" t="s">
-        <v>207</v>
       </c>
     </row>
     <row r="28" spans="1:9" s="4" customFormat="1" ht="21" x14ac:dyDescent="0.25">
@@ -4274,10 +4299,10 @@
       </c>
       <c r="E28" s="12"/>
       <c r="F28" s="12" t="s">
-        <v>215</v>
-      </c>
-      <c r="G28" s="12" t="s">
-        <v>217</v>
+        <v>214</v>
+      </c>
+      <c r="G28" s="19">
+        <v>45757</v>
       </c>
       <c r="H28" s="12" t="s">
         <v>147</v>
@@ -4293,23 +4318,23 @@
       </c>
       <c r="C29" s="12"/>
       <c r="D29" s="12" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="E29" s="12"/>
       <c r="F29" s="12" t="s">
+        <v>215</v>
+      </c>
+      <c r="G29" s="19">
+        <v>45757</v>
+      </c>
+      <c r="H29" s="12" t="s">
         <v>216</v>
       </c>
-      <c r="G29" s="12" t="s">
+      <c r="I29" s="12" t="s">
         <v>217</v>
       </c>
-      <c r="H29" s="12" t="s">
-        <v>218</v>
-      </c>
-      <c r="I29" s="12" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" s="4" customFormat="1" ht="21" x14ac:dyDescent="0.25">
+    </row>
+    <row r="30" spans="1:9" s="4" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A30" s="12" t="s">
         <v>103</v>
       </c>
@@ -4318,12 +4343,18 @@
       </c>
       <c r="C30" s="12"/>
       <c r="D30" s="12" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="E30" s="12"/>
-      <c r="F30" s="12"/>
-      <c r="G30" s="12"/>
-      <c r="H30" s="12"/>
+      <c r="F30" s="12" t="s">
+        <v>219</v>
+      </c>
+      <c r="G30" s="19">
+        <v>45758</v>
+      </c>
+      <c r="H30" s="12" t="s">
+        <v>147</v>
+      </c>
       <c r="I30" s="12"/>
     </row>
     <row r="31" spans="1:9" s="4" customFormat="1" ht="21" x14ac:dyDescent="0.25">
@@ -4338,10 +4369,18 @@
         <v>131</v>
       </c>
       <c r="E31" s="12"/>
-      <c r="F31" s="12"/>
-      <c r="G31" s="12"/>
-      <c r="H31" s="12"/>
-      <c r="I31" s="12"/>
+      <c r="F31" s="12" t="s">
+        <v>220</v>
+      </c>
+      <c r="G31" s="17" t="s">
+        <v>218</v>
+      </c>
+      <c r="H31" s="12" t="s">
+        <v>147</v>
+      </c>
+      <c r="I31" s="12" t="s">
+        <v>221</v>
+      </c>
     </row>
     <row r="32" spans="1:9" s="4" customFormat="1" ht="21" x14ac:dyDescent="0.25">
       <c r="A32" s="12" t="s">
@@ -4357,10 +4396,18 @@
       <c r="E32" s="12" t="s">
         <v>135</v>
       </c>
-      <c r="F32" s="12"/>
-      <c r="G32" s="12"/>
-      <c r="H32" s="12"/>
-      <c r="I32" s="12"/>
+      <c r="F32" s="12" t="s">
+        <v>223</v>
+      </c>
+      <c r="G32" s="17" t="s">
+        <v>218</v>
+      </c>
+      <c r="H32" s="12" t="s">
+        <v>178</v>
+      </c>
+      <c r="I32" s="12" t="s">
+        <v>222</v>
+      </c>
     </row>
     <row r="33" spans="1:9" s="4" customFormat="1" ht="21" x14ac:dyDescent="0.25">
       <c r="A33" s="12" t="s">
@@ -4377,7 +4424,7 @@
         <v>135</v>
       </c>
       <c r="F33" s="12"/>
-      <c r="G33" s="12"/>
+      <c r="G33" s="17"/>
       <c r="H33" s="12"/>
       <c r="I33" s="12"/>
     </row>
@@ -4396,7 +4443,7 @@
         <v>135</v>
       </c>
       <c r="F34" s="12"/>
-      <c r="G34" s="12"/>
+      <c r="G34" s="17"/>
       <c r="H34" s="12"/>
       <c r="I34" s="12"/>
     </row>
@@ -4413,7 +4460,7 @@
       </c>
       <c r="E35" s="12"/>
       <c r="F35" s="12"/>
-      <c r="G35" s="12"/>
+      <c r="G35" s="17"/>
       <c r="H35" s="12"/>
       <c r="I35" s="12"/>
     </row>
@@ -4430,7 +4477,7 @@
       </c>
       <c r="E36" s="12"/>
       <c r="F36" s="12"/>
-      <c r="G36" s="12"/>
+      <c r="G36" s="17"/>
       <c r="H36" s="12"/>
       <c r="I36" s="12"/>
     </row>
@@ -4447,7 +4494,7 @@
       </c>
       <c r="E37" s="12"/>
       <c r="F37" s="12"/>
-      <c r="G37" s="12"/>
+      <c r="G37" s="17"/>
       <c r="H37" s="12"/>
       <c r="I37" s="12"/>
     </row>
@@ -4462,7 +4509,7 @@
       <c r="D38" s="12"/>
       <c r="E38" s="12"/>
       <c r="F38" s="12"/>
-      <c r="G38" s="12"/>
+      <c r="G38" s="17"/>
       <c r="H38" s="12"/>
       <c r="I38" s="12"/>
     </row>
@@ -4477,13 +4524,13 @@
       <c r="D39" s="12"/>
       <c r="E39" s="12"/>
       <c r="F39" s="12"/>
-      <c r="G39" s="12"/>
+      <c r="G39" s="17"/>
       <c r="H39" s="12"/>
       <c r="I39" s="12"/>
     </row>
     <row r="40" spans="1:9" s="4" customFormat="1" ht="10.5" x14ac:dyDescent="0.25">
       <c r="A40" s="12" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B40" s="12" t="s">
         <v>128</v>
@@ -4492,13 +4539,13 @@
       <c r="D40" s="12"/>
       <c r="E40" s="12"/>
       <c r="F40" s="12"/>
-      <c r="G40" s="12"/>
+      <c r="G40" s="17"/>
       <c r="H40" s="12"/>
       <c r="I40" s="12"/>
     </row>
     <row r="41" spans="1:9" s="4" customFormat="1" ht="10.5" x14ac:dyDescent="0.25">
       <c r="A41" s="12" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B41" s="12" t="s">
         <v>128</v>
@@ -4507,7 +4554,7 @@
       <c r="D41" s="12"/>
       <c r="E41" s="12"/>
       <c r="F41" s="12"/>
-      <c r="G41" s="12"/>
+      <c r="G41" s="17"/>
       <c r="H41" s="12"/>
       <c r="I41" s="12"/>
     </row>

</xml_diff>

<commit_message>
chore(db, documentations) added database credentials and updated test documentations
</commit_message>
<xml_diff>
--- a/Documentation/Testplanering_Testfall.xlsx
+++ b/Documentation/Testplanering_Testfall.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Local\Peter\Testning\SecuremeTesting@fendraq\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87BF5DAA-D02C-48C3-A817-2333FC07C92A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2F793EA-48EE-4EFD-84E5-3AED070F4294}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" firstSheet="2" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="224">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="225">
   <si>
     <t>Test-ID</t>
   </si>
@@ -716,6 +716,9 @@
   </si>
   <si>
     <t>Kunden kan skriva ett meddelande som visas när sidan uppdateras.</t>
+  </si>
+  <si>
+    <t>Inget som hanterar open case eller sätter case handler</t>
   </si>
 </sst>
 </file>
@@ -908,15 +911,6 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
@@ -928,6 +922,15 @@
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3633,9 +3636,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A27" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F33" sqref="F33"/>
+      <selection pane="bottomLeft" activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3644,7 +3647,7 @@
     <col min="2" max="3" width="11.1796875" style="13" customWidth="1"/>
     <col min="4" max="5" width="27.453125" style="13" customWidth="1"/>
     <col min="6" max="6" width="25.6328125" style="13" customWidth="1"/>
-    <col min="7" max="7" width="11.1796875" style="20" customWidth="1"/>
+    <col min="7" max="7" width="11.1796875" style="17" customWidth="1"/>
     <col min="8" max="8" width="11.1796875" style="13" customWidth="1"/>
     <col min="9" max="9" width="42.26953125" style="13" customWidth="1"/>
   </cols>
@@ -3668,7 +3671,7 @@
       <c r="F1" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="18" t="s">
+      <c r="G1" s="15" t="s">
         <v>3</v>
       </c>
       <c r="H1" s="11" t="s">
@@ -3695,7 +3698,7 @@
       <c r="F2" s="12" t="s">
         <v>141</v>
       </c>
-      <c r="G2" s="17"/>
+      <c r="G2" s="14"/>
       <c r="H2" s="12"/>
       <c r="I2" s="12" t="s">
         <v>142</v>
@@ -3718,7 +3721,7 @@
       <c r="F3" s="12" t="s">
         <v>141</v>
       </c>
-      <c r="G3" s="17"/>
+      <c r="G3" s="14"/>
       <c r="H3" s="12"/>
       <c r="I3" s="12"/>
     </row>
@@ -3739,7 +3742,7 @@
       <c r="F4" s="12" t="s">
         <v>141</v>
       </c>
-      <c r="G4" s="17"/>
+      <c r="G4" s="14"/>
       <c r="H4" s="12"/>
       <c r="I4" s="12"/>
     </row>
@@ -3758,7 +3761,7 @@
       </c>
       <c r="E5" s="12"/>
       <c r="F5" s="12"/>
-      <c r="G5" s="17"/>
+      <c r="G5" s="14"/>
       <c r="H5" s="12"/>
       <c r="I5" s="12"/>
     </row>
@@ -3771,7 +3774,7 @@
       <c r="D6" s="12"/>
       <c r="E6" s="12"/>
       <c r="F6" s="12"/>
-      <c r="G6" s="17"/>
+      <c r="G6" s="14"/>
       <c r="H6" s="12"/>
       <c r="I6" s="12"/>
     </row>
@@ -3784,7 +3787,7 @@
       <c r="D7" s="12"/>
       <c r="E7" s="12"/>
       <c r="F7" s="12"/>
-      <c r="G7" s="17"/>
+      <c r="G7" s="14"/>
       <c r="H7" s="12"/>
       <c r="I7" s="12"/>
     </row>
@@ -3797,7 +3800,7 @@
       <c r="D8" s="12"/>
       <c r="E8" s="12"/>
       <c r="F8" s="12"/>
-      <c r="G8" s="17"/>
+      <c r="G8" s="14"/>
       <c r="H8" s="12"/>
       <c r="I8" s="12"/>
     </row>
@@ -3810,7 +3813,7 @@
       <c r="D9" s="12"/>
       <c r="E9" s="12"/>
       <c r="F9" s="12"/>
-      <c r="G9" s="17"/>
+      <c r="G9" s="14"/>
       <c r="H9" s="12"/>
       <c r="I9" s="12"/>
     </row>
@@ -3823,7 +3826,7 @@
       <c r="D10" s="12"/>
       <c r="E10" s="12"/>
       <c r="F10" s="12"/>
-      <c r="G10" s="17"/>
+      <c r="G10" s="14"/>
       <c r="H10" s="12"/>
       <c r="I10" s="12"/>
     </row>
@@ -3836,7 +3839,7 @@
       <c r="D11" s="12"/>
       <c r="E11" s="12"/>
       <c r="F11" s="12"/>
-      <c r="G11" s="17"/>
+      <c r="G11" s="14"/>
       <c r="H11" s="12"/>
       <c r="I11" s="12"/>
     </row>
@@ -3857,7 +3860,7 @@
         <v>173</v>
       </c>
       <c r="F12" s="12"/>
-      <c r="G12" s="17"/>
+      <c r="G12" s="14"/>
       <c r="H12" s="12" t="s">
         <v>178</v>
       </c>
@@ -3882,7 +3885,7 @@
       <c r="F13" s="12" t="s">
         <v>150</v>
       </c>
-      <c r="G13" s="17" t="s">
+      <c r="G13" s="14" t="s">
         <v>149</v>
       </c>
       <c r="H13" s="12" t="s">
@@ -3911,7 +3914,7 @@
       <c r="F14" s="12" t="s">
         <v>146</v>
       </c>
-      <c r="G14" s="17" t="s">
+      <c r="G14" s="14" t="s">
         <v>149</v>
       </c>
       <c r="H14" s="12" t="s">
@@ -3940,7 +3943,7 @@
       <c r="F15" s="12" t="s">
         <v>177</v>
       </c>
-      <c r="G15" s="17" t="s">
+      <c r="G15" s="14" t="s">
         <v>149</v>
       </c>
       <c r="H15" s="12" t="s">
@@ -3967,7 +3970,7 @@
       <c r="F16" s="12" t="s">
         <v>182</v>
       </c>
-      <c r="G16" s="17" t="s">
+      <c r="G16" s="14" t="s">
         <v>151</v>
       </c>
       <c r="H16" s="12" t="s">
@@ -3994,7 +3997,7 @@
       <c r="F17" s="12" t="s">
         <v>184</v>
       </c>
-      <c r="G17" s="17" t="s">
+      <c r="G17" s="14" t="s">
         <v>151</v>
       </c>
       <c r="H17" s="12" t="s">
@@ -4021,7 +4024,7 @@
       <c r="F18" s="12" t="s">
         <v>180</v>
       </c>
-      <c r="G18" s="17" t="s">
+      <c r="G18" s="14" t="s">
         <v>149</v>
       </c>
       <c r="H18" s="12" t="s">
@@ -4050,7 +4053,7 @@
       <c r="F19" s="12" t="s">
         <v>187</v>
       </c>
-      <c r="G19" s="17" t="s">
+      <c r="G19" s="14" t="s">
         <v>149</v>
       </c>
       <c r="H19" s="12" t="s">
@@ -4079,7 +4082,7 @@
       <c r="F20" s="12" t="s">
         <v>192</v>
       </c>
-      <c r="G20" s="17" t="s">
+      <c r="G20" s="14" t="s">
         <v>151</v>
       </c>
       <c r="H20" s="12" t="s">
@@ -4108,7 +4111,7 @@
       <c r="F21" s="12" t="s">
         <v>192</v>
       </c>
-      <c r="G21" s="17" t="s">
+      <c r="G21" s="14" t="s">
         <v>151</v>
       </c>
       <c r="H21" s="12" t="s">
@@ -4135,7 +4138,7 @@
       <c r="F22" s="12" t="s">
         <v>190</v>
       </c>
-      <c r="G22" s="17" t="s">
+      <c r="G22" s="14" t="s">
         <v>151</v>
       </c>
       <c r="H22" s="12" t="s">
@@ -4164,7 +4167,7 @@
       <c r="F23" s="12" t="s">
         <v>190</v>
       </c>
-      <c r="G23" s="17" t="s">
+      <c r="G23" s="14" t="s">
         <v>151</v>
       </c>
       <c r="H23" s="12" t="s">
@@ -4191,7 +4194,7 @@
       <c r="F24" s="12" t="s">
         <v>198</v>
       </c>
-      <c r="G24" s="17" t="s">
+      <c r="G24" s="14" t="s">
         <v>151</v>
       </c>
       <c r="H24" s="12" t="s">
@@ -4220,7 +4223,7 @@
       <c r="F25" s="12" t="s">
         <v>201</v>
       </c>
-      <c r="G25" s="19">
+      <c r="G25" s="16">
         <v>45756</v>
       </c>
       <c r="H25" s="12" t="s">
@@ -4249,7 +4252,7 @@
       <c r="F26" s="12" t="s">
         <v>203</v>
       </c>
-      <c r="G26" s="19">
+      <c r="G26" s="16">
         <v>45756</v>
       </c>
       <c r="H26" s="12" t="s">
@@ -4276,7 +4279,7 @@
       <c r="F27" s="12" t="s">
         <v>205</v>
       </c>
-      <c r="G27" s="19">
+      <c r="G27" s="16">
         <v>45756</v>
       </c>
       <c r="H27" s="12" t="s">
@@ -4301,7 +4304,7 @@
       <c r="F28" s="12" t="s">
         <v>214</v>
       </c>
-      <c r="G28" s="19">
+      <c r="G28" s="16">
         <v>45757</v>
       </c>
       <c r="H28" s="12" t="s">
@@ -4324,7 +4327,7 @@
       <c r="F29" s="12" t="s">
         <v>215</v>
       </c>
-      <c r="G29" s="19">
+      <c r="G29" s="16">
         <v>45757</v>
       </c>
       <c r="H29" s="12" t="s">
@@ -4349,7 +4352,7 @@
       <c r="F30" s="12" t="s">
         <v>219</v>
       </c>
-      <c r="G30" s="19">
+      <c r="G30" s="16">
         <v>45758</v>
       </c>
       <c r="H30" s="12" t="s">
@@ -4368,11 +4371,13 @@
       <c r="D31" s="12" t="s">
         <v>131</v>
       </c>
-      <c r="E31" s="12"/>
+      <c r="E31" s="12" t="s">
+        <v>224</v>
+      </c>
       <c r="F31" s="12" t="s">
         <v>220</v>
       </c>
-      <c r="G31" s="17" t="s">
+      <c r="G31" s="14" t="s">
         <v>218</v>
       </c>
       <c r="H31" s="12" t="s">
@@ -4399,7 +4404,7 @@
       <c r="F32" s="12" t="s">
         <v>223</v>
       </c>
-      <c r="G32" s="17" t="s">
+      <c r="G32" s="14" t="s">
         <v>218</v>
       </c>
       <c r="H32" s="12" t="s">
@@ -4424,7 +4429,7 @@
         <v>135</v>
       </c>
       <c r="F33" s="12"/>
-      <c r="G33" s="17"/>
+      <c r="G33" s="14"/>
       <c r="H33" s="12"/>
       <c r="I33" s="12"/>
     </row>
@@ -4443,7 +4448,7 @@
         <v>135</v>
       </c>
       <c r="F34" s="12"/>
-      <c r="G34" s="17"/>
+      <c r="G34" s="14"/>
       <c r="H34" s="12"/>
       <c r="I34" s="12"/>
     </row>
@@ -4460,7 +4465,7 @@
       </c>
       <c r="E35" s="12"/>
       <c r="F35" s="12"/>
-      <c r="G35" s="17"/>
+      <c r="G35" s="14"/>
       <c r="H35" s="12"/>
       <c r="I35" s="12"/>
     </row>
@@ -4477,7 +4482,7 @@
       </c>
       <c r="E36" s="12"/>
       <c r="F36" s="12"/>
-      <c r="G36" s="17"/>
+      <c r="G36" s="14"/>
       <c r="H36" s="12"/>
       <c r="I36" s="12"/>
     </row>
@@ -4494,7 +4499,7 @@
       </c>
       <c r="E37" s="12"/>
       <c r="F37" s="12"/>
-      <c r="G37" s="17"/>
+      <c r="G37" s="14"/>
       <c r="H37" s="12"/>
       <c r="I37" s="12"/>
     </row>
@@ -4509,7 +4514,7 @@
       <c r="D38" s="12"/>
       <c r="E38" s="12"/>
       <c r="F38" s="12"/>
-      <c r="G38" s="17"/>
+      <c r="G38" s="14"/>
       <c r="H38" s="12"/>
       <c r="I38" s="12"/>
     </row>
@@ -4524,7 +4529,7 @@
       <c r="D39" s="12"/>
       <c r="E39" s="12"/>
       <c r="F39" s="12"/>
-      <c r="G39" s="17"/>
+      <c r="G39" s="14"/>
       <c r="H39" s="12"/>
       <c r="I39" s="12"/>
     </row>
@@ -4539,7 +4544,7 @@
       <c r="D40" s="12"/>
       <c r="E40" s="12"/>
       <c r="F40" s="12"/>
-      <c r="G40" s="17"/>
+      <c r="G40" s="14"/>
       <c r="H40" s="12"/>
       <c r="I40" s="12"/>
     </row>
@@ -4554,7 +4559,7 @@
       <c r="D41" s="12"/>
       <c r="E41" s="12"/>
       <c r="F41" s="12"/>
-      <c r="G41" s="17"/>
+      <c r="G41" s="14"/>
       <c r="H41" s="12"/>
       <c r="I41" s="12"/>
     </row>
@@ -4584,18 +4589,18 @@
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A2" s="14" t="s">
+      <c r="A2" s="18" t="s">
         <v>197</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A3" s="15"/>
+      <c r="A3" s="19"/>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A4" s="15"/>
+      <c r="A4" s="19"/>
     </row>
     <row r="5" spans="1:1" ht="209.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="16"/>
+      <c r="A5" s="20"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
Testing and reports done
</commit_message>
<xml_diff>
--- a/Documentation/Testplanering_Testfall.xlsx
+++ b/Documentation/Testplanering_Testfall.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Local\Peter\Testning\SecuremeTesting@fendraq\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99A21ACD-DF9D-4F82-BDFE-FAEF6CFF5B85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FF7A99A-AF14-4308-B42A-26DC42D4734C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" firstSheet="2" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="12710" yWindow="0" windowWidth="12980" windowHeight="13770" firstSheet="2" activeTab="3" xr2:uid="{808F399E-ACB7-433E-85BA-137ADDF6E5A5}"/>
   </bookViews>
   <sheets>
     <sheet name="Kravspecifikationer" sheetId="2" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="307" uniqueCount="231">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="232">
   <si>
     <t>Test-ID</t>
   </si>
@@ -619,6 +619,114 @@
   </si>
   <si>
     <t>Skulle behöva en DTO som avgör hur mycket data som skickas till frontend. All data skickas nu. Det görs heller inget urval  om ett ärende är öppet eller inte. Stängda ärenden borde skickas via en egen API, Eftersom listan för varje medarbetare borde visa aktiva ärenden endast.</t>
+  </si>
+  <si>
+    <t>HTTP 201</t>
+  </si>
+  <si>
+    <t>Sucess / Refactor / Restrict</t>
+  </si>
+  <si>
+    <t>Användare skapas men returnerar ett objekt med all insatt data, inklusive lösenord. Bättre hade varit att ha ett objekt som returnerar success tillsammans med id, user_name, ev mejladress.</t>
+  </si>
+  <si>
+    <t>HTTP 200 + Uppdaterad beroende på vad som uppdateras.</t>
+  </si>
+  <si>
+    <t>Uppdaterar användare dynamiskt, att man alltså kan lägga till vilka värden som man vill ska uppdateras och utelämna andra. Däremot finns det ingen restriktion på att uppdatera vad som helst på användaren, så lösenord kan ändras utan problem. Om du däremot inte skickar med Active = true, ändras Active till false.</t>
+  </si>
+  <si>
+    <t>HTTP 500. Ska inte kunna gå att ta bort en användare, eftersom FK till cases</t>
+  </si>
+  <si>
+    <t>Onödig API för det ska inte gå att ta bort en användare från databasen. De ska kunna sättas inaktiva eller tas bort genom soft delete från frontend.</t>
+  </si>
+  <si>
+    <t>HTTP 200 + meddelande om ok</t>
+  </si>
+  <si>
+    <t>En användares möjlighet till att skapa ett eget lösenord fungerar, men eftersom databasen inte har unique på användare kan två användare med samma användarnamn uppdateras samtidigt men detta syns inte i responsen eftersom  samma meddelande skickas oavsett hur många rader som påverkas.</t>
+  </si>
+  <si>
+    <t>Skickar null-värden om kolumnen i databasen saknar värde eller inte är med i querien, exempel case_handler vid unopened och chatToken. Skickar för mycket data.</t>
+  </si>
+  <si>
+    <t>Success / Refactor / Restrict</t>
+  </si>
+  <si>
+    <t>Success /  Refactor / Restrict</t>
+  </si>
+  <si>
+    <t>TC-039</t>
+  </si>
+  <si>
+    <t>Verifiera att kundformuläret hanterar felaktig mejladress</t>
+  </si>
+  <si>
+    <t>TC-040</t>
+  </si>
+  <si>
+    <t>Verfiera att kundformuläret kräver fullständig information från kunden</t>
+  </si>
+  <si>
+    <t>Ett nytt ärende skapas och en alert med "Message sent successfully" visas.</t>
+  </si>
+  <si>
+    <t>Ett nytt ärende skapas inte och ett felmedelande genereras</t>
+  </si>
+  <si>
+    <t>Bug</t>
+  </si>
+  <si>
+    <t>Det ligger inga restriktioner om att inputdata måste vara i ett visst format i frontend. Däremot skickar backend meddelande om att mejl inte kunde skickas</t>
+  </si>
+  <si>
+    <t>2025-04-11</t>
+  </si>
+  <si>
+    <t>Ett nytt ärende skapas inte och ett felmeddelande genereras som informerar att alla fält är obligatoriska</t>
+  </si>
+  <si>
+    <t>En unik chatt öppnas för kunden</t>
+  </si>
+  <si>
+    <t>Behövs fler assertions?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lade till klassnamn för att lättare nå elementen. Men chatten uppdaterar inte automatiskt. </t>
+  </si>
+  <si>
+    <t>Kunden kan skriva ett meddelande som visas när sidan uppdateras.</t>
+  </si>
+  <si>
+    <t>Inget som hanterar open case eller sätter case handler</t>
+  </si>
+  <si>
+    <t>På Mina ärenden finns inte id utan behöver använda en selector på titel- Testet kan utvecklas för att se att det blir en lista. Behöver klassnamn</t>
+  </si>
+  <si>
+    <t>2025-04-16</t>
+  </si>
+  <si>
+    <t>My Cases-sidan syns och innehåller ärendet som visar chatten när det klickas på</t>
+  </si>
+  <si>
+    <t>Verifiera att kundtjänstmedarbetare kan se samma chatt som kunden</t>
+  </si>
+  <si>
+    <t>Verifiera att chatten uppdateras för kunden och kundtjänstmedarbetaren när de skickar meddelanden</t>
+  </si>
+  <si>
+    <t>Efter refresh kommer båda parterna se meddelandena.</t>
+  </si>
+  <si>
+    <t>Status ändras på det stängda ärendet.</t>
+  </si>
+  <si>
+    <t>Id och klassnamn saknas</t>
+  </si>
+  <si>
+    <t>Ignorerad så länge för får den inte att fungera</t>
   </si>
   <si>
     <t xml:space="preserve">- Inga restriktioner finns på API-endpoints eftersom autentisering saknas i projektet.
@@ -631,112 +739,10 @@
 - Tänkt lite fel. Session är implementerad i backend. Det är bara i frontend som den inte hanteras.
 - Detaljer i förhållande till säkerhet saknas i många fall: Exempel: inaktiv medarbetare kan logga in, skickar data till frontend som inte behövs (bla i ärendehantering), 
 - Inga restriktioner på API i förhållande till inloggad användare i session
+Frontend
+- I frontend ligger inga restriktioner på att input måste vara i ett visst format
+- Saknas mycket klassnamn och id. 
 - Lärdom: Att kritiskt granska och testa API så ser man hur man skulle kunna bygga upp en endpoint bättre, både genom vilken data som hämtas, returneras  och hur säkerheten ska hanteras exempelvis genom att låsa api till session och användare. </t>
-  </si>
-  <si>
-    <t>HTTP 201</t>
-  </si>
-  <si>
-    <t>Sucess / Refactor / Restrict</t>
-  </si>
-  <si>
-    <t>Användare skapas men returnerar ett objekt med all insatt data, inklusive lösenord. Bättre hade varit att ha ett objekt som returnerar success tillsammans med id, user_name, ev mejladress.</t>
-  </si>
-  <si>
-    <t>HTTP 200 + Uppdaterad beroende på vad som uppdateras.</t>
-  </si>
-  <si>
-    <t>Uppdaterar användare dynamiskt, att man alltså kan lägga till vilka värden som man vill ska uppdateras och utelämna andra. Däremot finns det ingen restriktion på att uppdatera vad som helst på användaren, så lösenord kan ändras utan problem. Om du däremot inte skickar med Active = true, ändras Active till false.</t>
-  </si>
-  <si>
-    <t>HTTP 500. Ska inte kunna gå att ta bort en användare, eftersom FK till cases</t>
-  </si>
-  <si>
-    <t>Onödig API för det ska inte gå att ta bort en användare från databasen. De ska kunna sättas inaktiva eller tas bort genom soft delete från frontend.</t>
-  </si>
-  <si>
-    <t>HTTP 200 + meddelande om ok</t>
-  </si>
-  <si>
-    <t>En användares möjlighet till att skapa ett eget lösenord fungerar, men eftersom databasen inte har unique på användare kan två användare med samma användarnamn uppdateras samtidigt men detta syns inte i responsen eftersom  samma meddelande skickas oavsett hur många rader som påverkas.</t>
-  </si>
-  <si>
-    <t>Skickar null-värden om kolumnen i databasen saknar värde eller inte är med i querien, exempel case_handler vid unopened och chatToken. Skickar för mycket data.</t>
-  </si>
-  <si>
-    <t>Success / Refactor / Restrict</t>
-  </si>
-  <si>
-    <t>Success /  Refactor / Restrict</t>
-  </si>
-  <si>
-    <t>TC-039</t>
-  </si>
-  <si>
-    <t>Verifiera att kundformuläret hanterar felaktig mejladress</t>
-  </si>
-  <si>
-    <t>TC-040</t>
-  </si>
-  <si>
-    <t>Verfiera att kundformuläret kräver fullständig information från kunden</t>
-  </si>
-  <si>
-    <t>Ett nytt ärende skapas och en alert med "Message sent successfully" visas.</t>
-  </si>
-  <si>
-    <t>Ett nytt ärende skapas inte och ett felmedelande genereras</t>
-  </si>
-  <si>
-    <t>Bug</t>
-  </si>
-  <si>
-    <t>Det ligger inga restriktioner om att inputdata måste vara i ett visst format i frontend. Däremot skickar backend meddelande om att mejl inte kunde skickas</t>
-  </si>
-  <si>
-    <t>2025-04-11</t>
-  </si>
-  <si>
-    <t>Ett nytt ärende skapas inte och ett felmeddelande genereras som informerar att alla fält är obligatoriska</t>
-  </si>
-  <si>
-    <t>En unik chatt öppnas för kunden</t>
-  </si>
-  <si>
-    <t>Behövs fler assertions?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Lade till klassnamn för att lättare nå elementen. Men chatten uppdaterar inte automatiskt. </t>
-  </si>
-  <si>
-    <t>Kunden kan skriva ett meddelande som visas när sidan uppdateras.</t>
-  </si>
-  <si>
-    <t>Inget som hanterar open case eller sätter case handler</t>
-  </si>
-  <si>
-    <t>På Mina ärenden finns inte id utan behöver använda en selector på titel- Testet kan utvecklas för att se att det blir en lista. Behöver klassnamn</t>
-  </si>
-  <si>
-    <t>2025-04-16</t>
-  </si>
-  <si>
-    <t>My Cases-sidan syns och innehåller ärendet som visar chatten när det klickas på</t>
-  </si>
-  <si>
-    <t>Verifiera att kundtjänstmedarbetare kan se samma chatt som kunden</t>
-  </si>
-  <si>
-    <t>Verifiera att chatten uppdateras för kunden och kundtjänstmedarbetaren när de skickar meddelanden</t>
-  </si>
-  <si>
-    <t>Efter refresh kommer båda parterna se meddelandena.</t>
-  </si>
-  <si>
-    <t>Status ändras på det stängda ärendet.</t>
-  </si>
-  <si>
-    <t>Id och klassnamn saknas</t>
   </si>
 </sst>
 </file>
@@ -1232,10 +1238,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CCEDDDBC-32B7-44BA-AAB9-3DFB4493A901}">
   <dimension ref="A1:A8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:A8"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -1291,10 +1294,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5464F935-DEAA-4EF7-8B39-9358828D74A1}">
   <dimension ref="A1:G39"/>
   <sheetViews>
-    <sheetView zoomScale="151" zoomScaleNormal="151" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2:A9"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -1699,10 +1699,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8469AB0C-99E3-4B57-8F81-DE8A23FADE51}">
   <dimension ref="A1:G39"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B19" sqref="B19"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -2107,10 +2104,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0DAC0F83-9806-4801-90A6-2FE0AA568BAD}">
   <dimension ref="A1:G40"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A18" sqref="A18"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -2527,10 +2521,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC31A750-71E8-4741-BD79-BC2E7283B985}">
   <dimension ref="A1:G39"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B17" sqref="B17"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -2901,10 +2892,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2806904-9931-468C-B904-ADB244BBE6B6}">
   <dimension ref="A1:G39"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2:A4"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -3277,10 +3265,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1EBD99A8-A7E2-4F91-A000-EBF798E7DFE7}">
   <dimension ref="A1:G39"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D17" sqref="D17"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -3654,9 +3639,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F39" sqref="F39"/>
+    <sheetView topLeftCell="A24" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="E1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3910,7 +3895,7 @@
         <v>176</v>
       </c>
       <c r="I13" s="12" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="14" spans="1:9" s="4" customFormat="1" ht="42" x14ac:dyDescent="0.25">
@@ -3965,7 +3950,7 @@
         <v>147</v>
       </c>
       <c r="H15" s="12" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="I15" s="12" t="s">
         <v>177</v>
@@ -4104,7 +4089,7 @@
         <v>149</v>
       </c>
       <c r="H20" s="12" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="I20" s="12" t="s">
         <v>189</v>
@@ -4160,7 +4145,7 @@
         <v>149</v>
       </c>
       <c r="H22" s="12" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="I22" s="12" t="s">
         <v>192</v>
@@ -4210,16 +4195,16 @@
       </c>
       <c r="E24" s="12"/>
       <c r="F24" s="12" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="G24" s="14" t="s">
         <v>149</v>
       </c>
       <c r="H24" s="12" t="s">
+        <v>196</v>
+      </c>
+      <c r="I24" s="12" t="s">
         <v>197</v>
-      </c>
-      <c r="I24" s="12" t="s">
-        <v>198</v>
       </c>
     </row>
     <row r="25" spans="1:9" s="4" customFormat="1" ht="52.5" x14ac:dyDescent="0.25">
@@ -4239,16 +4224,16 @@
         <v>126</v>
       </c>
       <c r="F25" s="12" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="G25" s="16">
         <v>45756</v>
       </c>
       <c r="H25" s="12" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="I25" s="12" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="26" spans="1:9" s="4" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
@@ -4268,7 +4253,7 @@
         <v>127</v>
       </c>
       <c r="F26" s="12" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="G26" s="16">
         <v>45756</v>
@@ -4277,7 +4262,7 @@
         <v>145</v>
       </c>
       <c r="I26" s="12" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="27" spans="1:9" s="4" customFormat="1" ht="52.5" x14ac:dyDescent="0.25">
@@ -4295,16 +4280,16 @@
       </c>
       <c r="E27" s="12"/>
       <c r="F27" s="12" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="G27" s="16">
         <v>45756</v>
       </c>
       <c r="H27" s="12" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="I27" s="12" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="28" spans="1:9" s="4" customFormat="1" ht="21" x14ac:dyDescent="0.25">
@@ -4320,7 +4305,7 @@
       </c>
       <c r="E28" s="12"/>
       <c r="F28" s="12" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="G28" s="16">
         <v>45757</v>
@@ -4339,20 +4324,20 @@
       </c>
       <c r="C29" s="12"/>
       <c r="D29" s="12" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="E29" s="12"/>
       <c r="F29" s="12" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="G29" s="16">
         <v>45757</v>
       </c>
       <c r="H29" s="12" t="s">
+        <v>213</v>
+      </c>
+      <c r="I29" s="12" t="s">
         <v>214</v>
-      </c>
-      <c r="I29" s="12" t="s">
-        <v>215</v>
       </c>
     </row>
     <row r="30" spans="1:9" s="4" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
@@ -4364,11 +4349,11 @@
       </c>
       <c r="C30" s="12"/>
       <c r="D30" s="12" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="E30" s="12"/>
       <c r="F30" s="12" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="G30" s="16">
         <v>45758</v>
@@ -4390,19 +4375,19 @@
         <v>131</v>
       </c>
       <c r="E31" s="12" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="F31" s="12" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="G31" s="14" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="H31" s="12" t="s">
         <v>145</v>
       </c>
       <c r="I31" s="12" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="32" spans="1:9" s="4" customFormat="1" ht="21" x14ac:dyDescent="0.25">
@@ -4420,16 +4405,16 @@
         <v>133</v>
       </c>
       <c r="F32" s="12" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="G32" s="14" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="H32" s="12" t="s">
         <v>176</v>
       </c>
       <c r="I32" s="12" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="33" spans="1:9" s="4" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
@@ -4441,22 +4426,22 @@
       </c>
       <c r="C33" s="12"/>
       <c r="D33" s="12" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="E33" s="12" t="s">
         <v>133</v>
       </c>
       <c r="F33" s="12" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="G33" s="14" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="H33" s="12" t="s">
         <v>176</v>
       </c>
       <c r="I33" s="12" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="34" spans="1:9" s="4" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
@@ -4468,22 +4453,22 @@
       </c>
       <c r="C34" s="12"/>
       <c r="D34" s="12" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="E34" s="12" t="s">
         <v>133</v>
       </c>
       <c r="F34" s="12" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="G34" s="14" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="H34" s="12" t="s">
         <v>176</v>
       </c>
       <c r="I34" s="12" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="35" spans="1:9" s="4" customFormat="1" ht="21" x14ac:dyDescent="0.25">
@@ -4499,11 +4484,13 @@
       </c>
       <c r="E35" s="12"/>
       <c r="F35" s="12" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="G35" s="14"/>
       <c r="H35" s="12"/>
-      <c r="I35" s="12"/>
+      <c r="I35" s="12" t="s">
+        <v>230</v>
+      </c>
     </row>
     <row r="36" spans="1:9" s="4" customFormat="1" ht="10.5" x14ac:dyDescent="0.25">
       <c r="A36" s="12" t="s">
@@ -4571,7 +4558,7 @@
     </row>
     <row r="40" spans="1:9" s="4" customFormat="1" ht="10.5" x14ac:dyDescent="0.25">
       <c r="A40" s="12" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B40" s="12" t="s">
         <v>128</v>
@@ -4586,7 +4573,7 @@
     </row>
     <row r="41" spans="1:9" s="4" customFormat="1" ht="10.5" x14ac:dyDescent="0.25">
       <c r="A41" s="12" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B41" s="12" t="s">
         <v>128</v>
@@ -4610,9 +4597,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{617D4732-2C37-4F78-B2EE-5A3CA7A21E97}">
   <dimension ref="A1:A5"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -4626,7 +4611,7 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A2" s="18" t="s">
-        <v>195</v>
+        <v>231</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.35">

</xml_diff>